<commit_message>
added validation for semester input for new lease request and added period to view invoice and view lease menu and updated related queries. Tested and working
</commit_message>
<xml_diff>
--- a/testCases.xlsx
+++ b/testCases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="216">
   <si>
     <t>Step</t>
   </si>
@@ -825,6 +825,18 @@
   </si>
   <si>
     <t>pass</t>
+  </si>
+  <si>
+    <t>one extra option - pay all invoices</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>works but formatting problem</t>
+  </si>
+  <si>
+    <t>does not display based on date</t>
   </si>
 </sst>
 </file>
@@ -995,24 +1007,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1038,6 +1032,24 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1343,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,60 +1379,63 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="13" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
       <c r="F3" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="F4" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="5"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1438,37 +1453,40 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
         <v>2.1</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
+    <row r="9" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="F9" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="6"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1482,64 +1500,67 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
         <v>3.1</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+      <c r="F13" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
       <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
       <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
       <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1553,865 +1574,901 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="15" t="s">
+      <c r="F21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="15" t="s">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="15" t="s">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
       <c r="B25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
       <c r="B26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="16"/>
       <c r="B27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-    </row>
-    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="16" t="s">
+    <row r="29" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+      <c r="B29" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-    </row>
-    <row r="30" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="16" t="s">
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="F29" t="s">
+        <v>211</v>
+      </c>
+      <c r="G29" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="B30" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-    </row>
-    <row r="31" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="17" t="s">
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="16"/>
+      <c r="B31" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-    </row>
-    <row r="32" spans="1:4" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+    </row>
+    <row r="32" spans="1:7" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
         <v>39</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
+      <c r="F32" t="s">
+        <v>213</v>
+      </c>
+      <c r="G32" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="16"/>
       <c r="B33" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-    </row>
-    <row r="34" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
         <v>43</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
+      <c r="F34" t="s">
+        <v>213</v>
+      </c>
+      <c r="G34" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
       <c r="B35" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-    </row>
-    <row r="36" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
       <c r="B36" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="F36" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
       <c r="B37" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
       <c r="B38" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="15"/>
       <c r="B39" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="16"/>
       <c r="B40" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-    </row>
-    <row r="41" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
         <v>50</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="15"/>
       <c r="B42" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="9"/>
+      <c r="C42" s="18"/>
       <c r="D42" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
+      <c r="F42" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="15"/>
       <c r="B43" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="13"/>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="16"/>
       <c r="B44" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="14"/>
-    </row>
-    <row r="45" spans="1:4" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+      <c r="C44" s="19"/>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="1:7" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
         <v>56</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7"/>
+      <c r="F45" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="16"/>
       <c r="B46" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-    </row>
-    <row r="47" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
         <v>59</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="15"/>
       <c r="B48" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-    </row>
-    <row r="49" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="15"/>
       <c r="B49" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="F49" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="15"/>
       <c r="B50" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="15"/>
       <c r="B51" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="7"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="16"/>
       <c r="B52" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-    </row>
-    <row r="53" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
         <v>64</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="15"/>
       <c r="B54" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-    </row>
-    <row r="55" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="15"/>
       <c r="B55" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="7"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="F55" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="16"/>
       <c r="B56" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-    </row>
-    <row r="57" spans="1:4" ht="153" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+    </row>
+    <row r="57" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
         <v>68</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="17" t="s">
         <v>77</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="15"/>
       <c r="B58" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="9"/>
+      <c r="C58" s="18"/>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="15"/>
       <c r="B59" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C59" s="9"/>
+      <c r="C59" s="18"/>
       <c r="D59" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="306" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
+    <row r="60" spans="1:6" ht="102" x14ac:dyDescent="0.25">
+      <c r="A60" s="15"/>
       <c r="B60" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C60" s="9"/>
-      <c r="D60" s="13"/>
-    </row>
-    <row r="61" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="7"/>
+    </row>
+    <row r="61" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="15"/>
       <c r="B61" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="13"/>
-    </row>
-    <row r="62" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="15"/>
       <c r="B62" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C62" s="9"/>
-      <c r="D62" s="13"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="7"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="15"/>
       <c r="B63" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C63" s="9"/>
-      <c r="D63" s="13"/>
-    </row>
-    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="7"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="7"/>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="16"/>
       <c r="B64" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C64" s="10"/>
-      <c r="D64" s="14"/>
-    </row>
-    <row r="65" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+      <c r="C64" s="19"/>
+      <c r="D64" s="8"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
         <v>79</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="D65" s="17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="15"/>
       <c r="B66" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-    </row>
-    <row r="67" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+    </row>
+    <row r="67" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="15"/>
       <c r="B67" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-    </row>
-    <row r="68" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="15"/>
       <c r="B68" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
+      <c r="A69" s="15"/>
       <c r="B69" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
     </row>
     <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="7"/>
+      <c r="A70" s="16"/>
       <c r="B70" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-    </row>
-    <row r="71" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
+      <c r="C70" s="19"/>
+      <c r="D70" s="19"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
         <v>84</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C71" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="D71" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="15"/>
       <c r="B72" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C72" s="9"/>
-      <c r="D72" s="9"/>
-    </row>
-    <row r="73" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="15"/>
       <c r="B73" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
     </row>
     <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="7"/>
+      <c r="A74" s="16"/>
       <c r="B74" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
     </row>
     <row r="75" spans="1:4" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
+      <c r="A75" s="14" t="s">
         <v>88</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C75" s="8" t="s">
+      <c r="C75" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D75" s="8" t="s">
+      <c r="D75" s="17" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="7"/>
+      <c r="A76" s="16"/>
       <c r="B76" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
-    </row>
-    <row r="77" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
+      <c r="C76" s="19"/>
+      <c r="D76" s="19"/>
+    </row>
+    <row r="77" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="14" t="s">
         <v>91</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="C77" s="17" t="s">
         <v>31</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
+    <row r="78" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="15"/>
       <c r="B78" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C78" s="9"/>
+      <c r="C78" s="18"/>
       <c r="D78" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="7"/>
+      <c r="A79" s="16"/>
       <c r="B79" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C79" s="10"/>
-      <c r="D79" s="14"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
+      <c r="A80" s="14" t="s">
         <v>96</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C80" s="8" t="s">
+      <c r="C80" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="D80" s="17" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="7"/>
+      <c r="A81" s="16"/>
       <c r="B81" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C81" s="10"/>
-      <c r="D81" s="10"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="19"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="11"/>
+      <c r="A82" s="5"/>
     </row>
     <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="11" t="s">
+      <c r="A83" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="6" t="s">
+    <row r="84" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A84" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B84" s="18" t="s">
+      <c r="B84" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="C84" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D84" s="18" t="s">
+      <c r="D84" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
+    <row r="85" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A85" s="15"/>
       <c r="B85" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C85" s="9"/>
+      <c r="C85" s="18"/>
       <c r="D85" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
+    <row r="86" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A86" s="15"/>
       <c r="B86" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C86" s="9"/>
-      <c r="D86" s="13"/>
-    </row>
-    <row r="87" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="7"/>
+    </row>
+    <row r="87" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="15"/>
       <c r="B87" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C87" s="9"/>
-      <c r="D87" s="13"/>
-    </row>
-    <row r="88" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="7"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="15"/>
       <c r="B88" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C88" s="9"/>
-      <c r="D88" s="13"/>
-    </row>
-    <row r="89" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="7"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="15"/>
       <c r="B89" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C89" s="9"/>
-      <c r="D89" s="13"/>
-    </row>
-    <row r="90" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="7"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="15"/>
       <c r="B90" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C90" s="9"/>
-      <c r="D90" s="13"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="7"/>
     </row>
     <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="7"/>
+      <c r="A91" s="16"/>
       <c r="B91" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C91" s="10"/>
-      <c r="D91" s="14"/>
-    </row>
-    <row r="92" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
+      <c r="C91" s="19"/>
+      <c r="D91" s="8"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="14" t="s">
         <v>110</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C92" s="8" t="s">
+      <c r="C92" s="17" t="s">
         <v>77</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="102" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
+    <row r="93" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A93" s="15"/>
       <c r="B93" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C93" s="9"/>
+      <c r="C93" s="18"/>
       <c r="D93" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
+    <row r="94" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A94" s="15"/>
       <c r="B94" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C94" s="9"/>
+      <c r="C94" s="18"/>
       <c r="D94" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="15"/>
       <c r="B95" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C95" s="9"/>
-      <c r="D95" s="13"/>
-    </row>
-    <row r="96" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A96" s="5"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="7"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="15"/>
       <c r="B96" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C96" s="9"/>
-      <c r="D96" s="13"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="7"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
+      <c r="A97" s="15"/>
       <c r="B97" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C97" s="9"/>
-      <c r="D97" s="13"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="7"/>
     </row>
     <row r="98" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="7"/>
+      <c r="A98" s="16"/>
       <c r="B98" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C98" s="10"/>
-      <c r="D98" s="14"/>
+      <c r="C98" s="19"/>
+      <c r="D98" s="8"/>
     </row>
     <row r="99" spans="1:4" ht="226.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="6" t="s">
+      <c r="A99" s="14" t="s">
         <v>118</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C99" s="8" t="s">
+      <c r="C99" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D99" s="8" t="s">
+      <c r="D99" s="17" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="7"/>
+      <c r="A100" s="16"/>
       <c r="B100" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
+      <c r="C100" s="19"/>
+      <c r="D100" s="19"/>
     </row>
     <row r="101" spans="1:4" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="6" t="s">
+      <c r="A101" s="14" t="s">
         <v>121</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C101" s="8" t="s">
+      <c r="C101" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D101" s="8" t="s">
+      <c r="D101" s="17" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="7"/>
+      <c r="A102" s="16"/>
       <c r="B102" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C102" s="10"/>
-      <c r="D102" s="10"/>
-    </row>
-    <row r="103" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A103" s="6" t="s">
+      <c r="C102" s="19"/>
+      <c r="D102" s="19"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="14" t="s">
         <v>124</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C103" s="8" t="s">
+      <c r="C103" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D103" s="8" t="s">
+      <c r="D103" s="17" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A104" s="5"/>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="15"/>
       <c r="B104" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C104" s="9"/>
-      <c r="D104" s="9"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
     </row>
     <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="7"/>
+      <c r="A105" s="16"/>
       <c r="B105" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C105" s="10"/>
-      <c r="D105" s="10"/>
-    </row>
-    <row r="106" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A106" s="6" t="s">
+      <c r="C105" s="19"/>
+      <c r="D105" s="19"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="14" t="s">
         <v>128</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C106" s="8" t="s">
+      <c r="C106" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D106" s="8" t="s">
+      <c r="D106" s="17" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A107" s="5"/>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="15"/>
       <c r="B107" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C107" s="9"/>
-      <c r="D107" s="9"/>
+      <c r="C107" s="18"/>
+      <c r="D107" s="18"/>
     </row>
     <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="7"/>
+      <c r="A108" s="16"/>
       <c r="B108" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C108" s="10"/>
-      <c r="D108" s="10"/>
+      <c r="C108" s="19"/>
+      <c r="D108" s="19"/>
     </row>
     <row r="109" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="6" t="s">
+      <c r="A109" s="14" t="s">
         <v>131</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C109" s="8" t="s">
+      <c r="C109" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D109" s="8" t="s">
+      <c r="D109" s="17" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="7"/>
+      <c r="A110" s="16"/>
       <c r="B110" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C110" s="10"/>
-      <c r="D110" s="10"/>
+      <c r="C110" s="19"/>
+      <c r="D110" s="19"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="11"/>
+      <c r="A111" s="5"/>
     </row>
     <row r="112" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="11" t="s">
+      <c r="A112" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>0</v>
       </c>
@@ -2425,145 +2482,145 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A114" s="6" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="B114" s="16" t="s">
+      <c r="B114" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C114" s="8" t="s">
+      <c r="C114" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D114" s="8" t="s">
+      <c r="D114" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A115" s="5"/>
-      <c r="B115" s="16" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="15"/>
+      <c r="B115" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="C115" s="9"/>
-      <c r="D115" s="9"/>
-    </row>
-    <row r="116" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="7"/>
-      <c r="B116" s="17" t="s">
+      <c r="C115" s="18"/>
+      <c r="D115" s="18"/>
+    </row>
+    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="16"/>
+      <c r="B116" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C116" s="10"/>
-      <c r="D116" s="10"/>
-    </row>
-    <row r="117" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A117" s="6" t="s">
+      <c r="C116" s="19"/>
+      <c r="D116" s="19"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="14" t="s">
         <v>138</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C117" s="8" t="s">
+      <c r="C117" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D117" s="8" t="s">
+      <c r="D117" s="17" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A118" s="5"/>
+    <row r="118" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="15"/>
       <c r="B118" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C118" s="9"/>
-      <c r="D118" s="9"/>
-    </row>
-    <row r="119" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="7"/>
+      <c r="C118" s="18"/>
+      <c r="D118" s="18"/>
+    </row>
+    <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="16"/>
       <c r="B119" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C119" s="10"/>
-      <c r="D119" s="10"/>
-    </row>
-    <row r="120" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A120" s="6" t="s">
+      <c r="C119" s="19"/>
+      <c r="D119" s="19"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="14" t="s">
         <v>143</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C120" s="8" t="s">
+      <c r="C120" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D120" s="8" t="s">
+      <c r="D120" s="17" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="5"/>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="15"/>
       <c r="B121" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C121" s="9"/>
-      <c r="D121" s="9"/>
-    </row>
-    <row r="122" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A122" s="5"/>
+      <c r="C121" s="18"/>
+      <c r="D121" s="18"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="15"/>
       <c r="B122" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C122" s="9"/>
-      <c r="D122" s="9"/>
+      <c r="C122" s="18"/>
+      <c r="D122" s="18"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="5"/>
+      <c r="A123" s="15"/>
       <c r="B123" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C123" s="9"/>
-      <c r="D123" s="9"/>
+      <c r="C123" s="18"/>
+      <c r="D123" s="18"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="5"/>
+      <c r="A124" s="15"/>
       <c r="B124" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C124" s="9"/>
-      <c r="D124" s="9"/>
+      <c r="C124" s="18"/>
+      <c r="D124" s="18"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="5"/>
+      <c r="A125" s="15"/>
       <c r="B125" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C125" s="9"/>
-      <c r="D125" s="9"/>
-    </row>
-    <row r="126" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A126" s="5"/>
+      <c r="C125" s="18"/>
+      <c r="D125" s="18"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="15"/>
       <c r="B126" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C126" s="9"/>
-      <c r="D126" s="9"/>
+      <c r="C126" s="18"/>
+      <c r="D126" s="18"/>
     </row>
     <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="7"/>
+      <c r="A127" s="16"/>
       <c r="B127" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
+      <c r="C127" s="19"/>
+      <c r="D127" s="19"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="11"/>
+      <c r="A128" s="5"/>
     </row>
     <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="11" t="s">
+      <c r="A129" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>0</v>
       </c>
@@ -2578,104 +2635,104 @@
       </c>
     </row>
     <row r="131" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="6" t="s">
+      <c r="A131" s="14" t="s">
         <v>150</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C131" s="8" t="s">
+      <c r="C131" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D131" s="8" t="s">
+      <c r="D131" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A132" s="5"/>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="15"/>
       <c r="B132" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C132" s="9"/>
-      <c r="D132" s="9"/>
+      <c r="C132" s="18"/>
+      <c r="D132" s="18"/>
     </row>
     <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="7"/>
+      <c r="A133" s="16"/>
       <c r="B133" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C133" s="10"/>
-      <c r="D133" s="10"/>
-    </row>
-    <row r="134" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A134" s="6" t="s">
+      <c r="C133" s="19"/>
+      <c r="D133" s="19"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="14" t="s">
         <v>154</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C134" s="8" t="s">
+      <c r="C134" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D134" s="8" t="s">
+      <c r="D134" s="17" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="318.75" x14ac:dyDescent="0.25">
-      <c r="A135" s="5"/>
+    <row r="135" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A135" s="15"/>
       <c r="B135" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C135" s="9"/>
-      <c r="D135" s="9"/>
+      <c r="C135" s="18"/>
+      <c r="D135" s="18"/>
     </row>
     <row r="136" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="7"/>
+      <c r="A136" s="16"/>
       <c r="B136" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C136" s="10"/>
-      <c r="D136" s="10"/>
-    </row>
-    <row r="137" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A137" s="6" t="s">
+      <c r="C136" s="19"/>
+      <c r="D136" s="19"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="14" t="s">
         <v>158</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C137" s="8" t="s">
+      <c r="C137" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D137" s="8" t="s">
+      <c r="D137" s="17" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="102" x14ac:dyDescent="0.25">
-      <c r="A138" s="5"/>
+    <row r="138" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A138" s="15"/>
       <c r="B138" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C138" s="9"/>
-      <c r="D138" s="9"/>
+      <c r="C138" s="18"/>
+      <c r="D138" s="18"/>
     </row>
     <row r="139" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="7"/>
+      <c r="A139" s="16"/>
       <c r="B139" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C139" s="10"/>
-      <c r="D139" s="10"/>
+      <c r="C139" s="19"/>
+      <c r="D139" s="19"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="11"/>
+      <c r="A140" s="5"/>
     </row>
     <row r="141" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="12" t="s">
+      <c r="A141" s="6" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>0</v>
       </c>
@@ -2689,376 +2746,376 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A143" s="6" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="14" t="s">
         <v>164</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C143" s="8" t="s">
+      <c r="C143" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D143" s="8" t="s">
+      <c r="D143" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A144" s="5"/>
+    <row r="144" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A144" s="15"/>
       <c r="B144" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C144" s="9"/>
-      <c r="D144" s="9"/>
-    </row>
-    <row r="145" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A145" s="5"/>
+      <c r="C144" s="18"/>
+      <c r="D144" s="18"/>
+    </row>
+    <row r="145" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A145" s="15"/>
       <c r="B145" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C145" s="9"/>
-      <c r="D145" s="9"/>
-    </row>
-    <row r="146" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A146" s="5"/>
+      <c r="C145" s="18"/>
+      <c r="D145" s="18"/>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="15"/>
       <c r="B146" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C146" s="9"/>
-      <c r="D146" s="9"/>
-    </row>
-    <row r="147" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A147" s="5"/>
+      <c r="C146" s="18"/>
+      <c r="D146" s="18"/>
+    </row>
+    <row r="147" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A147" s="15"/>
       <c r="B147" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C147" s="9"/>
-      <c r="D147" s="9"/>
+      <c r="C147" s="18"/>
+      <c r="D147" s="18"/>
     </row>
     <row r="148" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="7"/>
+      <c r="A148" s="16"/>
       <c r="B148" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C148" s="10"/>
-      <c r="D148" s="10"/>
-    </row>
-    <row r="149" spans="1:4" ht="204" x14ac:dyDescent="0.25">
-      <c r="A149" s="6" t="s">
+      <c r="C148" s="19"/>
+      <c r="D148" s="19"/>
+    </row>
+    <row r="149" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A149" s="14" t="s">
         <v>170</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C149" s="8" t="s">
+      <c r="C149" s="17" t="s">
         <v>31</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="A150" s="5"/>
+    <row r="150" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A150" s="15"/>
       <c r="B150" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C150" s="9"/>
+      <c r="C150" s="18"/>
       <c r="D150" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A151" s="5"/>
+    <row r="151" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A151" s="15"/>
       <c r="B151" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C151" s="9"/>
+      <c r="C151" s="18"/>
       <c r="D151" s="3" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="5"/>
+      <c r="A152" s="15"/>
       <c r="B152" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C152" s="9"/>
-      <c r="D152" s="13"/>
+      <c r="C152" s="18"/>
+      <c r="D152" s="7"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="5"/>
+      <c r="A153" s="15"/>
       <c r="B153" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C153" s="9"/>
-      <c r="D153" s="13"/>
+      <c r="C153" s="18"/>
+      <c r="D153" s="7"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="5"/>
+      <c r="A154" s="15"/>
       <c r="B154" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C154" s="9"/>
-      <c r="D154" s="13"/>
+      <c r="C154" s="18"/>
+      <c r="D154" s="7"/>
     </row>
     <row r="155" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="7"/>
+      <c r="A155" s="16"/>
       <c r="B155" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C155" s="10"/>
-      <c r="D155" s="14"/>
-    </row>
-    <row r="156" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A156" s="6" t="s">
+      <c r="C155" s="19"/>
+      <c r="D155" s="8"/>
+    </row>
+    <row r="156" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A156" s="14" t="s">
         <v>177</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C156" s="8" t="s">
+      <c r="C156" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D156" s="8"/>
-    </row>
-    <row r="157" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A157" s="5"/>
+      <c r="D156" s="17"/>
+    </row>
+    <row r="157" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A157" s="15"/>
       <c r="B157" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C157" s="9"/>
-      <c r="D157" s="9"/>
-    </row>
-    <row r="158" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A158" s="5"/>
+      <c r="C157" s="18"/>
+      <c r="D157" s="18"/>
+    </row>
+    <row r="158" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A158" s="15"/>
       <c r="B158" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C158" s="9"/>
-      <c r="D158" s="9"/>
+      <c r="C158" s="18"/>
+      <c r="D158" s="18"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="5"/>
+      <c r="A159" s="15"/>
       <c r="B159" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C159" s="9"/>
-      <c r="D159" s="9"/>
+      <c r="C159" s="18"/>
+      <c r="D159" s="18"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="5"/>
+      <c r="A160" s="15"/>
       <c r="B160" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C160" s="9"/>
-      <c r="D160" s="9"/>
+      <c r="C160" s="18"/>
+      <c r="D160" s="18"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="5"/>
+      <c r="A161" s="15"/>
       <c r="B161" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C161" s="9"/>
-      <c r="D161" s="9"/>
+      <c r="C161" s="18"/>
+      <c r="D161" s="18"/>
     </row>
     <row r="162" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="7"/>
+      <c r="A162" s="16"/>
       <c r="B162" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C162" s="10"/>
-      <c r="D162" s="10"/>
-    </row>
-    <row r="163" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="A163" s="6" t="s">
+      <c r="C162" s="19"/>
+      <c r="D162" s="19"/>
+    </row>
+    <row r="163" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A163" s="14" t="s">
         <v>181</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C163" s="8" t="s">
+      <c r="C163" s="17" t="s">
         <v>31</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A164" s="5"/>
+    <row r="164" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A164" s="15"/>
       <c r="B164" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C164" s="9"/>
+      <c r="C164" s="18"/>
       <c r="D164" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A165" s="5"/>
+    <row r="165" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A165" s="15"/>
       <c r="B165" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C165" s="9"/>
-      <c r="D165" s="13"/>
+      <c r="C165" s="18"/>
+      <c r="D165" s="7"/>
     </row>
     <row r="166" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="7"/>
+      <c r="A166" s="16"/>
       <c r="B166" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C166" s="10"/>
-      <c r="D166" s="14"/>
-    </row>
-    <row r="167" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A167" s="6" t="s">
+      <c r="C166" s="19"/>
+      <c r="D166" s="8"/>
+    </row>
+    <row r="167" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A167" s="14" t="s">
         <v>187</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C167" s="8" t="s">
+      <c r="C167" s="17" t="s">
         <v>31</v>
       </c>
       <c r="D167" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A168" s="5"/>
+    <row r="168" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A168" s="15"/>
       <c r="B168" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="C168" s="9"/>
+      <c r="C168" s="18"/>
       <c r="D168" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
-      <c r="A169" s="5"/>
+    <row r="169" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A169" s="15"/>
       <c r="B169" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C169" s="9"/>
+      <c r="C169" s="18"/>
       <c r="D169" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A170" s="5"/>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="15"/>
       <c r="B170" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C170" s="9"/>
-      <c r="D170" s="13"/>
+      <c r="C170" s="18"/>
+      <c r="D170" s="7"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="5"/>
+      <c r="A171" s="15"/>
       <c r="B171" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C171" s="9"/>
-      <c r="D171" s="13"/>
+      <c r="C171" s="18"/>
+      <c r="D171" s="7"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="5"/>
+      <c r="A172" s="15"/>
       <c r="B172" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C172" s="9"/>
-      <c r="D172" s="13"/>
+      <c r="C172" s="18"/>
+      <c r="D172" s="7"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="5"/>
+      <c r="A173" s="15"/>
       <c r="B173" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C173" s="9"/>
-      <c r="D173" s="13"/>
+      <c r="C173" s="18"/>
+      <c r="D173" s="7"/>
     </row>
     <row r="174" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="7"/>
+      <c r="A174" s="16"/>
       <c r="B174" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C174" s="10"/>
-      <c r="D174" s="14"/>
-    </row>
-    <row r="175" spans="1:4" ht="204" x14ac:dyDescent="0.25">
-      <c r="A175" s="6" t="s">
+      <c r="C174" s="19"/>
+      <c r="D174" s="8"/>
+    </row>
+    <row r="175" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A175" s="14" t="s">
         <v>193</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C175" s="8" t="s">
+      <c r="C175" s="17" t="s">
         <v>31</v>
       </c>
       <c r="D175" s="3" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="A176" s="5"/>
+    <row r="176" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A176" s="15"/>
       <c r="B176" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C176" s="9"/>
+      <c r="C176" s="18"/>
       <c r="D176" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A177" s="5"/>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="15"/>
       <c r="B177" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C177" s="9"/>
-      <c r="D177" s="13"/>
+      <c r="C177" s="18"/>
+      <c r="D177" s="7"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="5"/>
+      <c r="A178" s="15"/>
       <c r="B178" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C178" s="9"/>
-      <c r="D178" s="13"/>
+      <c r="C178" s="18"/>
+      <c r="D178" s="7"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="5"/>
+      <c r="A179" s="15"/>
       <c r="B179" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C179" s="9"/>
-      <c r="D179" s="13"/>
+      <c r="C179" s="18"/>
+      <c r="D179" s="7"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="5"/>
+      <c r="A180" s="15"/>
       <c r="B180" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C180" s="9"/>
-      <c r="D180" s="13"/>
+      <c r="C180" s="18"/>
+      <c r="D180" s="7"/>
     </row>
     <row r="181" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="7"/>
+      <c r="A181" s="16"/>
       <c r="B181" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C181" s="10"/>
-      <c r="D181" s="14"/>
+      <c r="C181" s="19"/>
+      <c r="D181" s="8"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="11"/>
+      <c r="A182" s="5"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="11" t="s">
+      <c r="A183" s="5" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="11"/>
-    </row>
-    <row r="185" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="5"/>
+    </row>
+    <row r="185" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>0</v>
       </c>
@@ -3072,95 +3129,163 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="6">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="14">
         <v>5</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C186" s="8" t="s">
+      <c r="C186" s="17" t="s">
         <v>31</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="102" x14ac:dyDescent="0.25">
-      <c r="A187" s="5"/>
+    <row r="187" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A187" s="15"/>
       <c r="B187" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C187" s="9"/>
+      <c r="C187" s="18"/>
       <c r="D187" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="7"/>
+      <c r="A188" s="16"/>
       <c r="B188" s="4"/>
-      <c r="C188" s="10"/>
-      <c r="D188" s="14"/>
-    </row>
-    <row r="189" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A189" s="6">
+      <c r="C188" s="19"/>
+      <c r="D188" s="8"/>
+    </row>
+    <row r="189" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A189" s="14">
         <v>5.0999999999999996</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C189" s="8" t="s">
+      <c r="C189" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D189" s="8" t="s">
+      <c r="D189" s="17" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A190" s="5"/>
+    <row r="190" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A190" s="15"/>
       <c r="B190" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C190" s="9"/>
-      <c r="D190" s="9"/>
-    </row>
-    <row r="191" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A191" s="5"/>
+      <c r="C190" s="18"/>
+      <c r="D190" s="18"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="15"/>
       <c r="B191" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C191" s="9"/>
-      <c r="D191" s="9"/>
-    </row>
-    <row r="192" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A192" s="5"/>
+      <c r="C191" s="18"/>
+      <c r="D191" s="18"/>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="15"/>
       <c r="B192" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C192" s="9"/>
-      <c r="D192" s="9"/>
+      <c r="C192" s="18"/>
+      <c r="D192" s="18"/>
     </row>
     <row r="193" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="7"/>
+      <c r="A193" s="16"/>
       <c r="B193" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C193" s="10"/>
-      <c r="D193" s="10"/>
+      <c r="C193" s="19"/>
+      <c r="D193" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="A186:A188"/>
-    <mergeCell ref="C186:C188"/>
-    <mergeCell ref="A189:A193"/>
-    <mergeCell ref="C189:C193"/>
-    <mergeCell ref="D189:D193"/>
-    <mergeCell ref="A163:A166"/>
-    <mergeCell ref="C163:C166"/>
-    <mergeCell ref="A167:A174"/>
-    <mergeCell ref="C167:C174"/>
-    <mergeCell ref="A175:A181"/>
-    <mergeCell ref="C175:C181"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="C21:C27"/>
+    <mergeCell ref="D21:D27"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="C34:C40"/>
+    <mergeCell ref="D34:D40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="C41:C44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="A57:A64"/>
+    <mergeCell ref="C57:C64"/>
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="C65:C70"/>
+    <mergeCell ref="D65:D70"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="D71:D74"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="D47:D52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="C53:C56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="A84:A91"/>
+    <mergeCell ref="C84:C91"/>
+    <mergeCell ref="A92:A98"/>
+    <mergeCell ref="C92:C98"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="A106:A108"/>
+    <mergeCell ref="C106:C108"/>
+    <mergeCell ref="D106:D108"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="D99:D100"/>
+    <mergeCell ref="A101:A102"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="D101:D102"/>
+    <mergeCell ref="A103:A105"/>
+    <mergeCell ref="C103:C105"/>
+    <mergeCell ref="D103:D105"/>
+    <mergeCell ref="A120:A127"/>
+    <mergeCell ref="C120:C127"/>
+    <mergeCell ref="D120:D127"/>
+    <mergeCell ref="A131:A133"/>
+    <mergeCell ref="C131:C133"/>
+    <mergeCell ref="D131:D133"/>
+    <mergeCell ref="A114:A116"/>
+    <mergeCell ref="C114:C116"/>
+    <mergeCell ref="D114:D116"/>
+    <mergeCell ref="A117:A119"/>
+    <mergeCell ref="C117:C119"/>
+    <mergeCell ref="D117:D119"/>
     <mergeCell ref="A143:A148"/>
     <mergeCell ref="C143:C148"/>
     <mergeCell ref="D143:D148"/>
@@ -3175,85 +3300,17 @@
     <mergeCell ref="A137:A139"/>
     <mergeCell ref="C137:C139"/>
     <mergeCell ref="D137:D139"/>
-    <mergeCell ref="A120:A127"/>
-    <mergeCell ref="C120:C127"/>
-    <mergeCell ref="D120:D127"/>
-    <mergeCell ref="A131:A133"/>
-    <mergeCell ref="C131:C133"/>
-    <mergeCell ref="D131:D133"/>
-    <mergeCell ref="A114:A116"/>
-    <mergeCell ref="C114:C116"/>
-    <mergeCell ref="D114:D116"/>
-    <mergeCell ref="A117:A119"/>
-    <mergeCell ref="C117:C119"/>
-    <mergeCell ref="D117:D119"/>
-    <mergeCell ref="A106:A108"/>
-    <mergeCell ref="C106:C108"/>
-    <mergeCell ref="D106:D108"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="D109:D110"/>
-    <mergeCell ref="D99:D100"/>
-    <mergeCell ref="A101:A102"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="D101:D102"/>
-    <mergeCell ref="A103:A105"/>
-    <mergeCell ref="C103:C105"/>
-    <mergeCell ref="D103:D105"/>
-    <mergeCell ref="A84:A91"/>
-    <mergeCell ref="C84:C91"/>
-    <mergeCell ref="A92:A98"/>
-    <mergeCell ref="C92:C98"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="D80:D81"/>
-    <mergeCell ref="A57:A64"/>
-    <mergeCell ref="C57:C64"/>
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="C65:C70"/>
-    <mergeCell ref="D65:D70"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="C71:C74"/>
-    <mergeCell ref="D71:D74"/>
-    <mergeCell ref="A47:A52"/>
-    <mergeCell ref="C47:C52"/>
-    <mergeCell ref="D47:D52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="C53:C56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="C34:C40"/>
-    <mergeCell ref="D34:D40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="C41:C44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="C21:C27"/>
-    <mergeCell ref="D21:D27"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A186:A188"/>
+    <mergeCell ref="C186:C188"/>
+    <mergeCell ref="A189:A193"/>
+    <mergeCell ref="C189:C193"/>
+    <mergeCell ref="D189:D193"/>
+    <mergeCell ref="A163:A166"/>
+    <mergeCell ref="C163:C166"/>
+    <mergeCell ref="A167:A174"/>
+    <mergeCell ref="C167:C174"/>
+    <mergeCell ref="A175:A181"/>
+    <mergeCell ref="C175:C181"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>